<commit_message>
Add md for Elveovervaakning
</commit_message>
<xml_diff>
--- a/Elveovervaakning_klima/Data/Elevoverv_trends_climate_1980-2019.xlsx (script 01).xlsx
+++ b/Elveovervaakning_klima/Data/Elevoverv_trends_climate_1980-2019.xlsx (script 01).xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t xml:space="preserve">Parameter</t>
   </si>
@@ -88,6 +88,51 @@
   </si>
   <si>
     <t xml:space="preserve">SN99370</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sum(precipitation_amount P1Y)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SN3780</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SN30000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SN30260</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SN43360</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SN44080</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SN46850</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SN51250</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SN57480</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SN63530</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SN66210</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SN68270</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SN78850</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SN96970</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SN99500</t>
   </si>
 </sst>
 </file>
@@ -915,7 +960,491 @@
     <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" t="n">
+        <v>1980</v>
+      </c>
+      <c r="D2" t="n">
+        <v>2019</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0.138958294570753</v>
+      </c>
+      <c r="F2" t="n">
+        <v>3.59615384615384</v>
+      </c>
+      <c r="G2" t="n">
+        <v>125.865384615385</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="n">
+        <v>1980</v>
+      </c>
+      <c r="D3" t="n">
+        <v>2019</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0.0673677916589717</v>
+      </c>
+      <c r="F3" t="n">
+        <v>4.02008620689655</v>
+      </c>
+      <c r="G3" t="n">
+        <v>140.703017241379</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="n">
+        <v>1983</v>
+      </c>
+      <c r="D4" t="n">
+        <v>2019</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0.146569514589274</v>
+      </c>
+      <c r="F4" t="n">
+        <v>3.49074074074074</v>
+      </c>
+      <c r="G4" t="n">
+        <v>122.175925925926</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" t="n">
+        <v>1980</v>
+      </c>
+      <c r="D5" t="n">
+        <v>2019</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0.876850699870331</v>
+      </c>
+      <c r="F5" t="n">
+        <v>-0.232812500000001</v>
+      </c>
+      <c r="G5" t="n">
+        <v>-8.14843750000005</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" t="n">
+        <v>1980</v>
+      </c>
+      <c r="D6" t="n">
+        <v>2015</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0.148946024378606</v>
+      </c>
+      <c r="F6" t="n">
+        <v>3.80347222222222</v>
+      </c>
+      <c r="G6" t="n">
+        <v>133.121527777778</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" t="n">
+        <v>1980</v>
+      </c>
+      <c r="D7" t="n">
+        <v>2019</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0.0236392119138704</v>
+      </c>
+      <c r="F7" t="n">
+        <v>9.14074074074074</v>
+      </c>
+      <c r="G7" t="n">
+        <v>319.925925925926</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" t="n">
+        <v>1980</v>
+      </c>
+      <c r="D8" t="n">
+        <v>2019</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0.147464391575845</v>
+      </c>
+      <c r="F8" t="n">
+        <v>6.5</v>
+      </c>
+      <c r="G8" t="n">
+        <v>227.5</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" t="n">
+        <v>1980</v>
+      </c>
+      <c r="D9" t="n">
+        <v>2017</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0.365371548508621</v>
+      </c>
+      <c r="F9" t="n">
+        <v>3.48235294117646</v>
+      </c>
+      <c r="G9" t="n">
+        <v>121.882352941176</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" t="n">
+        <v>1980</v>
+      </c>
+      <c r="D10" t="n">
+        <v>2019</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0.711571463676106</v>
+      </c>
+      <c r="F10" t="n">
+        <v>1.18181818181818</v>
+      </c>
+      <c r="G10" t="n">
+        <v>41.3636363636364</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" t="n">
+        <v>1980</v>
+      </c>
+      <c r="D11" t="n">
+        <v>2019</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0.0994828152565819</v>
+      </c>
+      <c r="F11" t="n">
+        <v>12.9318181818182</v>
+      </c>
+      <c r="G11" t="n">
+        <v>452.613636363636</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12" t="n">
+        <v>1980</v>
+      </c>
+      <c r="D12" t="n">
+        <v>2019</v>
+      </c>
+      <c r="E12" t="n">
+        <v>0.392612310375168</v>
+      </c>
+      <c r="F12" t="n">
+        <v>8.42962962962963</v>
+      </c>
+      <c r="G12" t="n">
+        <v>295.037037037037</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13" t="n">
+        <v>1980</v>
+      </c>
+      <c r="D13" t="n">
+        <v>2019</v>
+      </c>
+      <c r="E13" t="n">
+        <v>0.506620569504461</v>
+      </c>
+      <c r="F13" t="n">
+        <v>4.22999999999997</v>
+      </c>
+      <c r="G13" t="n">
+        <v>148.049999999999</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" t="n">
+        <v>1980</v>
+      </c>
+      <c r="D14" t="n">
+        <v>2019</v>
+      </c>
+      <c r="E14" t="n">
+        <v>0.476729058288446</v>
+      </c>
+      <c r="F14" t="n">
+        <v>-1.76666666666667</v>
+      </c>
+      <c r="G14" t="n">
+        <v>-61.8333333333335</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" t="s">
+        <v>35</v>
+      </c>
+      <c r="C15" t="n">
+        <v>1980</v>
+      </c>
+      <c r="D15" t="n">
+        <v>2009</v>
+      </c>
+      <c r="E15" t="n">
+        <v>0.914752339084737</v>
+      </c>
+      <c r="F15" t="n">
+        <v>1.30000000000001</v>
+      </c>
+      <c r="G15" t="n">
+        <v>45.5000000000002</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16" t="s">
+        <v>36</v>
+      </c>
+      <c r="C16" t="n">
+        <v>1980</v>
+      </c>
+      <c r="D16" t="n">
+        <v>2019</v>
+      </c>
+      <c r="E16" t="n">
+        <v>0.345305697448102</v>
+      </c>
+      <c r="F16" t="n">
+        <v>2.58684210526317</v>
+      </c>
+      <c r="G16" t="n">
+        <v>90.539473684211</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>25</v>
+      </c>
+      <c r="B17" t="s">
+        <v>37</v>
+      </c>
+      <c r="C17" t="n">
+        <v>1980</v>
+      </c>
+      <c r="D17" t="n">
+        <v>2007</v>
+      </c>
+      <c r="E17" t="n">
+        <v>0.243762192173415</v>
+      </c>
+      <c r="F17" t="n">
+        <v>9.04166666666667</v>
+      </c>
+      <c r="G17" t="n">
+        <v>316.458333333333</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>25</v>
+      </c>
+      <c r="B18" t="s">
+        <v>21</v>
+      </c>
+      <c r="C18" t="n">
+        <v>1980</v>
+      </c>
+      <c r="D18" t="n">
+        <v>2019</v>
+      </c>
+      <c r="E18" t="n">
+        <v>0.301495521705862</v>
+      </c>
+      <c r="F18" t="n">
+        <v>1.52290969899666</v>
+      </c>
+      <c r="G18" t="n">
+        <v>53.301839464883</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>25</v>
+      </c>
+      <c r="B19" t="s">
+        <v>22</v>
+      </c>
+      <c r="C19" t="n">
+        <v>1980</v>
+      </c>
+      <c r="D19" t="n">
+        <v>2017</v>
+      </c>
+      <c r="E19" t="n">
+        <v>0.0242392703746717</v>
+      </c>
+      <c r="F19" t="n">
+        <v>3.38928571428571</v>
+      </c>
+      <c r="G19" t="n">
+        <v>118.625</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>25</v>
+      </c>
+      <c r="B20" t="s">
+        <v>38</v>
+      </c>
+      <c r="C20" t="n">
+        <v>1980</v>
+      </c>
+      <c r="D20" t="n">
+        <v>2018</v>
+      </c>
+      <c r="E20" t="n">
+        <v>0.798239812457203</v>
+      </c>
+      <c r="F20" t="n">
+        <v>0.445161290322581</v>
+      </c>
+      <c r="G20" t="n">
+        <v>15.5806451612903</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>25</v>
+      </c>
+      <c r="B21" t="s">
+        <v>39</v>
+      </c>
+      <c r="C21" t="n">
+        <v>1980</v>
+      </c>
+      <c r="D21" t="n">
+        <v>2019</v>
+      </c>
+      <c r="E21" t="n">
+        <v>0.406443337928541</v>
+      </c>
+      <c r="F21" t="n">
+        <v>0.697142857142857</v>
+      </c>
+      <c r="G21" t="n">
+        <v>24.4</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>

</xml_diff>